<commit_message>
Invoke All Workflow File
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RPA\MY Project\Generate Yearly Report\REF_Generate-Yearly-Report-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64182AE0-6C27-46AC-84D6-53DA957DF30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -159,14 +159,62 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>ACME_Client</t>
+  </si>
+  <si>
+    <t>REF_Generate Yearly Report_Performer</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Year_Report</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>ACME_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>ACME_Workitem_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/</t>
+  </si>
+  <si>
+    <t>Download Monthly Report_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reports/download/</t>
+  </si>
+  <si>
+    <t>Upload Yearly Report_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reports/upload/</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Report_Data_Download</t>
+  </si>
+  <si>
+    <t>Data\Report\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -186,6 +234,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -211,15 +272,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -239,9 +305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -598,7 +664,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -618,30 +686,87 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="23.4">
+      <c r="A11" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.4"/>
+    <row r="18" spans="1:2" ht="23.4">
+      <c r="A18" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1599,15 +1724,6 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1620,7 +1736,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1670,7 +1786,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>25</v>
@@ -2782,7 +2898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
fix Select Item Month
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RPA\MY Project\Generate Yearly Report\REF_Generate-Yearly-Report-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF701093-803D-4CB5-9944-778FAD8F7F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3C5009-763A-4564-B8AF-DEC2DBDFA346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ACME_Client</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>REFDemo</t>
+  </si>
+  <si>
+    <t>ACME_NEW</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" activeCellId="1" sqref="B2:B3 C15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -654,7 +654,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -665,7 +665,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
@@ -688,15 +688,15 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="7">
         <v>2023</v>
@@ -704,54 +704,54 @@
     </row>
     <row r="11" spans="1:26" ht="23.4">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.4"/>
     <row r="18" spans="1:2" ht="23.4">
       <c r="A18" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
         <v>58</v>
-      </c>
-      <c r="B19" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>